<commit_message>
Add Cover Letter Page to WBS
</commit_message>
<xml_diff>
--- a/Definition/Design/High Level/WBS.xlsx
+++ b/Definition/Design/High Level/WBS.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mostafa Abdel Hamid\Desktop\workshop utomtion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eng. Nada\Desktop\bank\Internet-Banking-System-QA\Definition\Design\High Level\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{653B6154-12AB-4D85-8643-6AE3BE79C5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WBS Tree Diagram - BLANK" sheetId="4" r:id="rId1"/>
@@ -19,11 +18,11 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'WBS Tree Diagram - BLANK'!$B$1:$H$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'WBS Tree Diagram - BLANK'!$B$1:$H$21</definedName>
     <definedName name="Type" localSheetId="0">'[1]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,56 +32,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>PROJECT TITLE</t>
-  </si>
-  <si>
-    <t>PROJECT MANAGER</t>
-  </si>
-  <si>
-    <t>COMPANY NAME</t>
-  </si>
-  <si>
-    <t>WORK BREAKDOWN STRUCTURE TREE DIAGRAM TEMPLATE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Internet Banking System</t>
-  </si>
-  <si>
-    <t>Osama</t>
-  </si>
-  <si>
-    <t>ITI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -107,38 +72,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -155,39 +93,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Californian FB"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -195,109 +115,27 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -309,7 +147,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="9" xr:uid="{FBFF094A-0F25-DD4D-BCBE-4B7CA27D0685}"/>
+    <cellStyle name="Normal 2" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -329,22 +167,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:colOff>1114425</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>120135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>91560</xdr:rowOff>
+      <xdr:colOff>1114425</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>43936</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F0A5E48-6389-954A-9627-9E8CF51081E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F0A5E48-6389-954A-9627-9E8CF51081E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -352,8 +190,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9734550" y="2053710"/>
-          <a:ext cx="0" cy="381000"/>
+          <a:off x="9603581" y="6823354"/>
+          <a:ext cx="0" cy="376238"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -384,22 +222,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>690820</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>547945</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>41276</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{971A0B51-E8B0-1841-BBBD-B057D3705030}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{971A0B51-E8B0-1841-BBBD-B057D3705030}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -407,8 +245,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2995870" y="2428875"/>
-          <a:ext cx="16997105" cy="3175"/>
+          <a:off x="2857758" y="7193757"/>
+          <a:ext cx="17028061" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -439,22 +277,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>692150</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>692150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>197644</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DF9A586-827F-624F-A739-D164A65F04F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DF9A586-827F-624F-A739-D164A65F04F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -462,8 +300,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2997200" y="2438400"/>
-          <a:ext cx="0" cy="381000"/>
+          <a:off x="2859088" y="7203282"/>
+          <a:ext cx="0" cy="376237"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -494,22 +332,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>192645</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133114</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>511175</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{710BDE43-66AD-3C4E-811E-B8263184BF79}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{710BDE43-66AD-3C4E-811E-B8263184BF79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -517,8 +355,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="752475" y="3678795"/>
-          <a:ext cx="6350" cy="378855"/>
+          <a:off x="611981" y="8419864"/>
+          <a:ext cx="6350" cy="385999"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -549,22 +387,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1225550</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>202170</xdr:rowOff>
+      <xdr:colOff>1082675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142639</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1225550</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>128279</xdr:rowOff>
+      <xdr:colOff>1082675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>80654</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE913842-0144-2C4A-BF86-585078D9B237}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE913842-0144-2C4A-BF86-585078D9B237}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -572,8 +410,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5588000" y="3688320"/>
-          <a:ext cx="0" cy="383309"/>
+          <a:off x="5452269" y="8429389"/>
+          <a:ext cx="0" cy="390453"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -604,22 +442,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>682625</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>219869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>682625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>193675</xdr:rowOff>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>134144</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEB2B54C-EF98-7548-976D-DD235CC831EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DEB2B54C-EF98-7548-976D-DD235CC831EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -627,8 +465,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2987675" y="3298825"/>
-          <a:ext cx="0" cy="381000"/>
+          <a:off x="2849563" y="8054182"/>
+          <a:ext cx="0" cy="366712"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -659,22 +497,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>87312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>87313</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3130390F-17AF-E040-B23D-C2A445E7C21F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3130390F-17AF-E040-B23D-C2A445E7C21F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -682,8 +520,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="790575" y="4559300"/>
-          <a:ext cx="0" cy="685800"/>
+          <a:off x="650081" y="9302750"/>
+          <a:ext cx="0" cy="678657"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -714,22 +552,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>140494</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90AC4472-B42D-AF45-8D19-F4F3297AB3CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{90AC4472-B42D-AF45-8D19-F4F3297AB3CF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -737,8 +575,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="762000" y="3667125"/>
-          <a:ext cx="4819650" cy="19050"/>
+          <a:off x="621506" y="8420100"/>
+          <a:ext cx="4824413" cy="7144"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -765,22 +603,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>184883</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>102578</xdr:rowOff>
+      <xdr:colOff>42008</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>54954</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>184883</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>26377</xdr:rowOff>
+      <xdr:colOff>42008</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>204971</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="31" name="Straight Connector 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C60C71AC-7A1E-804B-BA14-DD2E11AA1272}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C60C71AC-7A1E-804B-BA14-DD2E11AA1272}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -788,8 +626,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12787191" y="2447193"/>
-          <a:ext cx="0" cy="378069"/>
+          <a:off x="12650727" y="7210610"/>
+          <a:ext cx="0" cy="376236"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -820,22 +658,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>558556</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>80840</xdr:rowOff>
+      <xdr:colOff>415681</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33216</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>558556</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>4639</xdr:rowOff>
+      <xdr:colOff>415681</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>183233</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="35" name="Straight Connector 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63373685-853B-7D45-B110-CEEB8E4B7BE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63373685-853B-7D45-B110-CEEB8E4B7BE4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -843,8 +681,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15468844" y="2425455"/>
-          <a:ext cx="0" cy="378069"/>
+          <a:off x="15334212" y="7188872"/>
+          <a:ext cx="0" cy="376236"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -875,22 +713,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1241425</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
+      <xdr:colOff>1169988</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>113506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1241425</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
+      <xdr:colOff>1169988</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>113507</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="40" name="TextBox 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20E83B1D-7E56-B14E-80E6-B98A47182F3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20E83B1D-7E56-B14E-80E6-B98A47182F3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -898,8 +736,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7661275" y="1577975"/>
-          <a:ext cx="4114800" cy="457200"/>
+          <a:off x="7599363" y="6364287"/>
+          <a:ext cx="4119563" cy="452439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -969,22 +807,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1425575</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>53975</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
+      <xdr:colOff>1282700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>194469</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1970881</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>194469</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="41" name="TextBox 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F79D18C-EFE1-B443-997E-D35D30C67BA3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F79D18C-EFE1-B443-997E-D35D30C67BA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -992,8 +830,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1673225" y="2816225"/>
-          <a:ext cx="2743200" cy="457200"/>
+          <a:off x="1532731" y="7576344"/>
+          <a:ext cx="2747963" cy="452438"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1083,22 +921,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1381125</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="42" name="TextBox 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F923B23-215D-3745-A0FA-00A7E738C6D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F923B23-215D-3745-A0FA-00A7E738C6D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1106,8 +944,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="142875" y="4016375"/>
-          <a:ext cx="1485900" cy="527050"/>
+          <a:off x="0" y="8764588"/>
+          <a:ext cx="1488281" cy="522287"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1173,22 +1011,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>390524</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="44" name="TextBox 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1392D049-DC61-1047-AD4D-CC71E842247B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1392D049-DC61-1047-AD4D-CC71E842247B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1196,8 +1034,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4752974" y="4057650"/>
-          <a:ext cx="1895475" cy="523876"/>
+          <a:off x="4617243" y="8805863"/>
+          <a:ext cx="1897856" cy="519113"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1311,22 +1149,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>168519</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>25644</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1381124</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>111124</xdr:rowOff>
+      <xdr:colOff>1238249</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="45" name="TextBox 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{366668F4-AB7C-BC44-B683-ADC2140BA7EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{366668F4-AB7C-BC44-B683-ADC2140BA7EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1334,8 +1172,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="417634" y="5251206"/>
-          <a:ext cx="1212605" cy="1314937"/>
+          <a:off x="275675" y="10003632"/>
+          <a:ext cx="1212605" cy="1311274"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1443,22 +1281,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1655884</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>1513009</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1222377</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>58616</xdr:rowOff>
+      <xdr:colOff>1079502</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>118147</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="47" name="TextBox 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F715320-9397-0242-83E9-9C369C1B17DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F715320-9397-0242-83E9-9C369C1B17DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1466,8 +1304,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3963865" y="6559794"/>
-          <a:ext cx="1625358" cy="2423014"/>
+          <a:off x="3822822" y="11308557"/>
+          <a:ext cx="1626274" cy="2418434"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1829,22 +1667,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1704976</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>1562101</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1476376</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>1333501</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>207169</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="70" name="TextBox 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9F309D3-2E20-4BEB-99B1-D78413AC04DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9F309D3-2E20-4BEB-99B1-D78413AC04DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1852,8 +1690,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4010026" y="5429250"/>
-          <a:ext cx="1828800" cy="619125"/>
+          <a:off x="3871914" y="10186988"/>
+          <a:ext cx="1831181" cy="592931"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1918,23 +1756,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2021681</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>202407</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2021681</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="74" name="Straight Connector 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E748FA44-7CBB-4D3F-9A02-AC41F55A4BAD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E748FA44-7CBB-4D3F-9A02-AC41F55A4BAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1942,8 +1780,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4467225" y="4905375"/>
-          <a:ext cx="0" cy="536575"/>
+          <a:off x="4331494" y="9644063"/>
+          <a:ext cx="0" cy="555625"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1974,22 +1812,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1647825</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>1504950</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1047750</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="90" name="TextBox 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4CDC3D4-5BD3-4D80-872A-B849CE65B536}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4CDC3D4-5BD3-4D80-872A-B849CE65B536}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1997,8 +1835,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6010275" y="5419725"/>
-          <a:ext cx="1457325" cy="552450"/>
+          <a:off x="5874544" y="10177463"/>
+          <a:ext cx="1459706" cy="528637"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2064,22 +1902,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1409700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="92" name="TextBox 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5100C3DF-D8B4-4CCB-9DC5-C332A858D2F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5100C3DF-D8B4-4CCB-9DC5-C332A858D2F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2087,8 +1925,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7829550" y="5429249"/>
-          <a:ext cx="1514475" cy="542925"/>
+          <a:off x="7696200" y="10186987"/>
+          <a:ext cx="1516856" cy="519112"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2177,23 +2015,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2002631</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>173832</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>192882</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="101" name="Straight Connector 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D9BD24F-6A4B-4708-8DB8-59214F461CCF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D9BD24F-6A4B-4708-8DB8-59214F461CCF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2201,8 +2039,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4448175" y="4876800"/>
-          <a:ext cx="6286500" cy="19050"/>
+          <a:off x="4312444" y="9615488"/>
+          <a:ext cx="6293644" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2229,22 +2067,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1428750</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>197644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>754672</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>21981</xdr:rowOff>
+      <xdr:colOff>611797</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>33887</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="105" name="TextBox 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB320DBD-58E5-4C1C-8809-50DF0835B87B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB320DBD-58E5-4C1C-8809-50DF0835B87B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2252,8 +2090,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7854462" y="6474069"/>
-          <a:ext cx="1384787" cy="1138604"/>
+          <a:off x="7715250" y="11222832"/>
+          <a:ext cx="1385703" cy="1134024"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2394,22 +2232,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>207169</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>60326</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="107" name="Straight Connector 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FA4ECB1-79D2-430C-A999-F7F716740A69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2FA4ECB1-79D2-430C-A999-F7F716740A69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2417,8 +2255,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4524375" y="6048375"/>
-          <a:ext cx="0" cy="536575"/>
+          <a:off x="4388644" y="10779919"/>
+          <a:ext cx="0" cy="531813"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2449,22 +2287,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1495425</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>216693</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1012825</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>869950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="113" name="TextBox 112">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{506337B2-5920-4689-ADDE-668CBF599CB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{506337B2-5920-4689-ADDE-668CBF599CB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2472,8 +2310,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5862271" y="6493118"/>
-          <a:ext cx="1576266" cy="1097574"/>
+          <a:off x="5722144" y="11241881"/>
+          <a:ext cx="1577181" cy="1092994"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2575,22 +2413,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1238250</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>187325</xdr:rowOff>
+      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>106362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>211932</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="117" name="Straight Connector 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C356F0E-D81C-4628-941E-B2A6C85B1C4A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C356F0E-D81C-4628-941E-B2A6C85B1C4A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2598,8 +2436,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5600700" y="4587875"/>
-          <a:ext cx="9525" cy="327025"/>
+          <a:off x="5464969" y="9321800"/>
+          <a:ext cx="9525" cy="331788"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2630,22 +2468,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>740020</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:colOff>597145</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>140494</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="132" name="TextBox 131">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5890AD2-7E3B-410C-A622-865C7B84EDC0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5890AD2-7E3B-410C-A622-865C7B84EDC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2653,8 +2491,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9627577" y="5392614"/>
-          <a:ext cx="1655885" cy="581026"/>
+          <a:off x="9489281" y="10167937"/>
+          <a:ext cx="1656802" cy="545307"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2720,22 +2558,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1581150</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1514475</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="134" name="TextBox 133">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC2B163A-D717-488E-9DEC-34255860A5F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EC2B163A-D717-488E-9DEC-34255860A5F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2743,8 +2581,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10058400" y="6543675"/>
-          <a:ext cx="1990725" cy="2019300"/>
+          <a:off x="9927431" y="11270457"/>
+          <a:ext cx="1993107" cy="2016918"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2897,22 +2735,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>575896</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>150393</xdr:rowOff>
+      <xdr:colOff>433021</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>102768</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>579071</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>116498</xdr:rowOff>
+      <xdr:colOff>436196</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>68873</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="143" name="Straight Connector 142">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C373304A-B3ED-491B-81DB-5305DD22E852}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C373304A-B3ED-491B-81DB-5305DD22E852}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2920,8 +2758,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="15486184" y="3176412"/>
-          <a:ext cx="3175" cy="420374"/>
+          <a:off x="15351552" y="7937081"/>
+          <a:ext cx="3175" cy="418542"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2951,23 +2789,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>8792</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1925698</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>542192</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:colOff>399317</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="144" name="TextBox 143">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E80DB018-A98D-4C1A-AA6F-516CD9481CFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E80DB018-A98D-4C1A-AA6F-516CD9481CFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2975,8 +2813,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14669965" y="2714625"/>
-          <a:ext cx="1603131" cy="454270"/>
+          <a:off x="14534417" y="7477125"/>
+          <a:ext cx="1604963" cy="452439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3049,22 +2887,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1945542</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>124558</xdr:rowOff>
+      <xdr:colOff>1802667</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1948961</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>103611</xdr:rowOff>
+      <xdr:colOff>1806086</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>55986</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="149" name="Straight Connector 148">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C101CE0C-2872-44D0-83F3-F74427E35058}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C101CE0C-2872-44D0-83F3-F74427E35058}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3072,8 +2910,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="14547850" y="3604846"/>
-          <a:ext cx="3419" cy="433323"/>
+          <a:off x="14411386" y="8363683"/>
+          <a:ext cx="3419" cy="431491"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3104,22 +2942,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268165</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>91585</xdr:rowOff>
+      <xdr:colOff>125290</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>43960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>572965</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>205886</xdr:rowOff>
+      <xdr:colOff>430090</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>122542</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="150" name="TextBox 149">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D16F3F58-74E1-4E28-B2B4-0D1AE77EB749}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D16F3F58-74E1-4E28-B2B4-0D1AE77EB749}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3127,8 +2965,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15999069" y="4026143"/>
-          <a:ext cx="1125415" cy="341435"/>
+          <a:off x="15865353" y="8783148"/>
+          <a:ext cx="1126331" cy="328613"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3209,22 +3047,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>153866</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>131884</xdr:rowOff>
+      <xdr:colOff>10991</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>60447</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>696059</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>102576</xdr:rowOff>
+      <xdr:colOff>553184</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>54951</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="151" name="TextBox 150">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{193A39D7-98D5-4666-AC7F-F7D834A57B34}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{193A39D7-98D5-4666-AC7F-F7D834A57B34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3232,8 +3070,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15884770" y="4747846"/>
-          <a:ext cx="1362808" cy="1582615"/>
+          <a:off x="15751054" y="9502103"/>
+          <a:ext cx="1363724" cy="1578036"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3313,7 +3151,7 @@
             </a:rPr>
             <a:t>transefer money 3.2.5 transaction  History</a:t>
           </a:r>
-          <a:endParaRPr lang="en-001" sz="900">
+          <a:endParaRPr lang="x-none" sz="900">
             <a:effectLst/>
             <a:latin typeface="Californian FB" panose="0207040306080B030204" pitchFamily="18" charset="0"/>
           </a:endParaRPr>
@@ -3325,22 +3163,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1406769</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>162658</xdr:rowOff>
+      <xdr:colOff>1263894</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>91221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>512885</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>109903</xdr:rowOff>
+      <xdr:colOff>370010</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>62278</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="156" name="TextBox 155">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A144A953-8D45-48DB-898E-7C8E9F04FF2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A144A953-8D45-48DB-898E-7C8E9F04FF2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3348,8 +3186,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14009077" y="4778620"/>
-          <a:ext cx="1414096" cy="1559168"/>
+          <a:off x="13872613" y="9532877"/>
+          <a:ext cx="1415928" cy="1554589"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3463,22 +3301,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1463918</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>93784</xdr:rowOff>
+      <xdr:colOff>1321043</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>46159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>273293</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>130418</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="159" name="TextBox 158">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6130E39C-FCE6-4EDB-9367-6D5B75FCAE8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6130E39C-FCE6-4EDB-9367-6D5B75FCAE8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3486,8 +3324,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14066226" y="4028342"/>
-          <a:ext cx="1117355" cy="360485"/>
+          <a:off x="13929762" y="8785347"/>
+          <a:ext cx="1119187" cy="358653"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3568,22 +3406,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1951892</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>131885</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>124558</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>146539</xdr:rowOff>
+      <xdr:colOff>1809017</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>84260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>803214</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>98914</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="162" name="Straight Connector 161">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A1A6105-308B-4C33-9FB2-0C504D316D39}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A1A6105-308B-4C33-9FB2-0C504D316D39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3591,8 +3429,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14554200" y="3612173"/>
-          <a:ext cx="2121877" cy="14654"/>
+          <a:off x="14417736" y="8371010"/>
+          <a:ext cx="2125541" cy="14654"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3618,23 +3456,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>112102</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161193</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>117231</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>82061</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>790758</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>113568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>795887</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>34436</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="166" name="Straight Connector 165">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C9F0A4-7E93-49AB-818B-843E50E201E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E5C9F0A4-7E93-49AB-818B-843E50E201E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3642,8 +3480,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="16663621" y="3641481"/>
-          <a:ext cx="5129" cy="375138"/>
+          <a:off x="16530821" y="8400318"/>
+          <a:ext cx="5129" cy="373306"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3674,22 +3512,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1981200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>226402</xdr:rowOff>
+      <xdr:colOff>1838325</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>143058</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1981200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152510</xdr:rowOff>
+      <xdr:colOff>1838325</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>81073</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="168" name="Straight Connector 167">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE9856BF-83C0-4D95-95B3-63F121D6D748}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CE9856BF-83C0-4D95-95B3-63F121D6D748}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3697,8 +3535,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14583508" y="4388094"/>
-          <a:ext cx="0" cy="380378"/>
+          <a:off x="14447044" y="9132277"/>
+          <a:ext cx="0" cy="390452"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3728,23 +3566,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>140678</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>198561</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>140678</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>124669</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>819334</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>115217</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>819334</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>53232</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="169" name="Straight Connector 168">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{377C17B4-2E3F-4A40-8399-9F56E760252A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{377C17B4-2E3F-4A40-8399-9F56E760252A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3752,8 +3590,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16692197" y="4360253"/>
-          <a:ext cx="0" cy="380378"/>
+          <a:off x="16559397" y="9104436"/>
+          <a:ext cx="0" cy="390452"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3784,22 +3622,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>402981</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>183906</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>36636</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>139212</xdr:rowOff>
+      <xdr:colOff>260106</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>136281</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>715292</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91587</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="187" name="TextBox 186">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9BDC314-C51B-49F2-97DE-3D5543B647B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9BDC314-C51B-49F2-97DE-3D5543B647B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3807,8 +3645,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19416346" y="2755656"/>
-          <a:ext cx="1274886" cy="409575"/>
+          <a:off x="19286294" y="7518156"/>
+          <a:ext cx="1276717" cy="407744"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3878,22 +3716,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>490171</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76444</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>347296</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>219807</xdr:rowOff>
+      <xdr:rowOff>28819</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>773906</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>136464</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="188" name="TextBox 187">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27CDD8E1-59A4-494D-827B-7BB62DF723C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{27CDD8E1-59A4-494D-827B-7BB62DF723C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3901,8 +3739,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19503536" y="3556732"/>
-          <a:ext cx="1246310" cy="1279037"/>
+          <a:off x="19373484" y="8315569"/>
+          <a:ext cx="1248141" cy="1262551"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4043,22 +3881,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>194162</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>139211</xdr:rowOff>
+      <xdr:colOff>51287</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>194162</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>65320</xdr:rowOff>
+      <xdr:colOff>51287</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>17695</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="189" name="Straight Connector 188">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BB475F3-25CC-4CA7-B3FE-8C86D369290B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2BB475F3-25CC-4CA7-B3FE-8C86D369290B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4066,8 +3904,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20028143" y="3165230"/>
-          <a:ext cx="0" cy="380378"/>
+          <a:off x="19899006" y="7925899"/>
+          <a:ext cx="0" cy="378546"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4098,22 +3936,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>181707</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>80596</xdr:rowOff>
+      <xdr:colOff>38832</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>32972</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>181707</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>174380</xdr:rowOff>
+      <xdr:colOff>38832</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>126755</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="198" name="Straight Connector 197">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F96199E3-2F0F-4721-B775-AB087583738A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F96199E3-2F0F-4721-B775-AB087583738A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4121,8 +3959,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20015688" y="2425211"/>
-          <a:ext cx="0" cy="320919"/>
+          <a:off x="19886551" y="7188628"/>
+          <a:ext cx="0" cy="320002"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4153,22 +3991,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>130969</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>682625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>112155</xdr:rowOff>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>64530</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="66" name="Straight Connector 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D70CEE-2E35-49A7-B3F2-D07299EFDAE0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20D70CEE-2E35-49A7-B3F2-D07299EFDAE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4176,8 +4014,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2981325" y="3676650"/>
-          <a:ext cx="6350" cy="378855"/>
+          <a:off x="2843213" y="8417719"/>
+          <a:ext cx="6350" cy="385999"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4208,22 +4046,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>156605</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>156605</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85168</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="68" name="Straight Connector 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94E2BFC5-AB32-4290-8B1C-784D01D1D555}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{94E2BFC5-AB32-4290-8B1C-784D01D1D555}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4231,8 +4069,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3019425" y="4557155"/>
-          <a:ext cx="0" cy="685800"/>
+          <a:off x="2881313" y="9300605"/>
+          <a:ext cx="0" cy="678657"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4262,23 +4100,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1983582</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>23255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>70880</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1552575</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>140730</xdr:rowOff>
+      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>69292</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="69" name="TextBox 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BA3DE8B-BF52-4216-9708-B7E4AF092060}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3BA3DE8B-BF52-4216-9708-B7E4AF092060}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4286,8 +4124,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2371725" y="4014230"/>
-          <a:ext cx="1485900" cy="527050"/>
+          <a:off x="2233613" y="8762443"/>
+          <a:ext cx="1485900" cy="522287"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4353,22 +4191,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>234461</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>91586</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>82549</xdr:rowOff>
+      <xdr:colOff>1228725</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="71" name="TextBox 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BC06771-9B73-46D2-85D9-48BBFA8AFB7B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2BC06771-9B73-46D2-85D9-48BBFA8AFB7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4376,8 +4214,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2542442" y="5222631"/>
-          <a:ext cx="1137139" cy="1314937"/>
+          <a:off x="2401399" y="9975057"/>
+          <a:ext cx="1137139" cy="1311274"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4506,22 +4344,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>173832</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="73" name="Straight Connector 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A1B85DF-2146-4778-9E5C-C0FCDB7A0647}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A1B85DF-2146-4778-9E5C-C0FCDB7A0647}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4529,8 +4367,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6677025" y="4876800"/>
-          <a:ext cx="0" cy="536575"/>
+          <a:off x="6543675" y="9615488"/>
+          <a:ext cx="0" cy="555625"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4561,22 +4399,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>130969</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>219869</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="75" name="Straight Connector 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D57DF77B-E6C9-48BA-B1F9-53CCBB78CCE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D57DF77B-E6C9-48BA-B1F9-53CCBB78CCE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4584,8 +4422,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6657975" y="5981700"/>
-          <a:ext cx="0" cy="536575"/>
+          <a:off x="6524625" y="10703719"/>
+          <a:ext cx="0" cy="541338"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4615,23 +4453,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>126024</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>30774</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>126024</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>110149</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2042930</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>185556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2042930</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>62524</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="76" name="Straight Connector 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC0AB30E-87ED-40DA-AB23-C23096676BFA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EC0AB30E-87ED-40DA-AB23-C23096676BFA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4639,8 +4477,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8610601" y="4873870"/>
-          <a:ext cx="0" cy="533644"/>
+          <a:off x="8472305" y="9627212"/>
+          <a:ext cx="0" cy="555625"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4671,22 +4509,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>170717</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>173648</xdr:rowOff>
+      <xdr:colOff>27842</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>126023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>170717</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>24423</xdr:rowOff>
+      <xdr:colOff>27842</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>203017</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="79" name="Straight Connector 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEA15EB9-84D3-44B7-AE44-2857949BA7BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEA15EB9-84D3-44B7-AE44-2857949BA7BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4694,8 +4532,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8655294" y="5947263"/>
-          <a:ext cx="0" cy="532179"/>
+          <a:off x="8516998" y="10698773"/>
+          <a:ext cx="0" cy="529432"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4726,22 +4564,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>164307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="80" name="Straight Connector 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDF914E3-7D19-4CD2-935F-C6FB757B3CF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FDF914E3-7D19-4CD2-935F-C6FB757B3CF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4749,8 +4587,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10744200" y="4867275"/>
-          <a:ext cx="0" cy="536575"/>
+          <a:off x="10615613" y="9605963"/>
+          <a:ext cx="0" cy="555625"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4781,22 +4619,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>150019</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>60325</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>12701</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="81" name="Straight Connector 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D91C2C3D-01F0-482D-9C4B-86A51B894885}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D91C2C3D-01F0-482D-9C4B-86A51B894885}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4804,8 +4642,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10753725" y="6000750"/>
-          <a:ext cx="0" cy="536575"/>
+          <a:off x="10625138" y="10722769"/>
+          <a:ext cx="0" cy="541338"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4836,22 +4674,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>214190</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>39513</xdr:rowOff>
+      <xdr:colOff>71315</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>218107</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>214190</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>194222</xdr:rowOff>
+      <xdr:colOff>71315</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>134691</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="83" name="Straight Connector 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BA24FF9-0C58-4593-B82A-63DB734C4D3F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5BA24FF9-0C58-4593-B82A-63DB734C4D3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4859,8 +4697,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12816498" y="3292667"/>
-          <a:ext cx="0" cy="381843"/>
+          <a:off x="12680034" y="8052420"/>
+          <a:ext cx="0" cy="369021"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4891,22 +4729,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1674202</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>53242</xdr:rowOff>
+      <xdr:colOff>1531327</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>5617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>740752</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>53243</xdr:rowOff>
+      <xdr:colOff>597877</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>5619</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="84" name="TextBox 83">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28EE0166-9989-4979-A80A-89A86D8BEFD7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{28EE0166-9989-4979-A80A-89A86D8BEFD7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4914,8 +4752,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12217644" y="2852127"/>
-          <a:ext cx="1125416" cy="454270"/>
+          <a:off x="12080265" y="7613711"/>
+          <a:ext cx="1126331" cy="452439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4972,22 +4810,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>707781</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>106974</xdr:rowOff>
+      <xdr:colOff>564906</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>59349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1899872</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>29308</xdr:rowOff>
+      <xdr:colOff>1756997</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>184089</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="85" name="TextBox 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D564F8-CE8B-4716-9FFF-E98281E15FA2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{71D564F8-CE8B-4716-9FFF-E98281E15FA2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4995,8 +4833,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11251223" y="4041532"/>
-          <a:ext cx="1192091" cy="376603"/>
+          <a:off x="11113844" y="8798537"/>
+          <a:ext cx="1192091" cy="374771"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5061,22 +4899,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1276350</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>181708</xdr:rowOff>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>134083</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>864577</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>197827</xdr:rowOff>
+      <xdr:colOff>721702</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>138296</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="91" name="Straight Connector 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F1722FD-3034-4B09-B6C6-3C76643AD746}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5F1722FD-3034-4B09-B6C6-3C76643AD746}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5084,8 +4922,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11819792" y="3661996"/>
-          <a:ext cx="1647093" cy="16119"/>
+          <a:off x="11682413" y="8420833"/>
+          <a:ext cx="1648008" cy="4213"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -5111,23 +4949,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1968195</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>84259</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>51289</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>131884</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1243380</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>54218</xdr:rowOff>
+      <xdr:colOff>1100505</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>208999</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="93" name="TextBox 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA9C396-8334-49C8-B005-AE7BAACD0D15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0CA9C396-8334-49C8-B005-AE7BAACD0D15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5135,8 +4973,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12653597" y="4066442"/>
-          <a:ext cx="1192091" cy="376603"/>
+          <a:off x="12517133" y="8823447"/>
+          <a:ext cx="1192091" cy="374771"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5221,22 +5059,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1282212</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>183174</xdr:rowOff>
+      <xdr:colOff>1139337</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>135549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1282212</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>110747</xdr:rowOff>
+      <xdr:colOff>1139337</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>63122</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="95" name="Straight Connector 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC19085-F4DB-4F0B-82E0-95744CCFAFA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8CC19085-F4DB-4F0B-82E0-95744CCFAFA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5244,8 +5082,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11825654" y="3663462"/>
-          <a:ext cx="0" cy="381843"/>
+          <a:off x="11688275" y="8422299"/>
+          <a:ext cx="0" cy="380011"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -5276,22 +5114,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>864577</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>721702</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>130969</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>864577</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>118073</xdr:rowOff>
+      <xdr:colOff>721702</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>70448</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="97" name="Straight Connector 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D33D0B0F-5634-45A2-BA59-266444B1DC4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D33D0B0F-5634-45A2-BA59-266444B1DC4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5299,8 +5137,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13466885" y="3670788"/>
-          <a:ext cx="0" cy="381843"/>
+          <a:off x="13330421" y="8417719"/>
+          <a:ext cx="0" cy="391917"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -5326,6 +5164,44 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1077825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1142999</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47157</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5447419" y="0"/>
+          <a:ext cx="8304299" cy="5393063"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5610,110 +5486,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA21F6B-F5BA-CA44-853D-BD3BFC4BD270}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H33"/>
+  <dimension ref="C1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="3" customWidth="1"/>
-    <col min="2" max="8" width="27" style="3" customWidth="1"/>
-    <col min="9" max="9" width="3.25" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.75" style="3"/>
+    <col min="1" max="1" width="3.25" style="1" customWidth="1"/>
+    <col min="2" max="8" width="27" style="1" customWidth="1"/>
+    <col min="9" max="9" width="3.25" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="10" t="s">
+    <row r="1" spans="3:8" ht="317.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:8" ht="51" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="7">
-        <v>44663</v>
-      </c>
-      <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="2:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
+    <row r="12" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14"/>
     </row>
-    <row r="14" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F16"/>
+    <row r="15" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
     </row>
-    <row r="17" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="11"/>
+    <row r="16" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="3"/>
+      <c r="H16" s="4"/>
     </row>
-    <row r="18" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="12"/>
-      <c r="H18" s="14"/>
-    </row>
-    <row r="19" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="3:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="66" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>